<commit_message>
Update Get Goodle Drive Links For Tio Cash.xlsx
</commit_message>
<xml_diff>
--- a/Get Goodle Drive Links For Tio Cash.xlsx
+++ b/Get Goodle Drive Links For Tio Cash.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PrimeSuspects\PrimeSuspects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABC72C2-3BF6-4A67-83B4-1A35BE00749C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A70541-E1D7-4F01-AB63-9E5352DFC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-129" yWindow="-129" windowWidth="22200" windowHeight="12600" activeTab="2" xr2:uid="{C13C5CDF-2E38-40E1-8BC5-5C2E79B9EFDA}"/>
   </bookViews>
@@ -2963,8 +2963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D779E8E-3A17-4982-94CC-39845AEB5192}">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O63" workbookViewId="0">
-      <selection activeCell="O72" sqref="O72"/>
+    <sheetView tabSelected="1" topLeftCell="I23" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.899999999999999" x14ac:dyDescent="0.65"/>

</xml_diff>